<commit_message>
se aumento mas  consultas
</commit_message>
<xml_diff>
--- a/mapeo.xlsx
+++ b/mapeo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\base de datos proyectos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\base de datos proyectos\base-de-datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04338564-3DA0-4A53-A5A7-834CAC84E311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C991818F-6C18-48EF-9258-2AA87E080809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -686,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="68" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N51" sqref="N51"/>
+    <sheetView topLeftCell="A27" zoomScale="68" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60:C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1423,210 +1423,6 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>71</v>
-      </c>
-      <c r="E47" t="s">
-        <v>85</v>
-      </c>
-      <c r="L47" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="M49" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="N49" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="O49" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="P49" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A50" s="3">
-        <v>111</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" s="3">
-        <v>7102020</v>
-      </c>
-      <c r="E50" s="3">
-        <v>100</v>
-      </c>
-      <c r="F50" s="3">
-        <v>10</v>
-      </c>
-      <c r="G50" s="6">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H50" s="3">
-        <v>1000</v>
-      </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="L50" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="M50" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="N50" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="E51" s="3">
-        <v>110</v>
-      </c>
-      <c r="F51" s="3">
-        <v>15</v>
-      </c>
-      <c r="G51" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="H51" s="3">
-        <v>1300</v>
-      </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="L51" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="M51" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="E52" s="3">
-        <v>111</v>
-      </c>
-      <c r="F52" s="3">
-        <v>16</v>
-      </c>
-      <c r="G52" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="H52" s="3">
-        <v>1200</v>
-      </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="E53" s="3">
-        <v>115</v>
-      </c>
-      <c r="F53" s="3">
-        <v>20</v>
-      </c>
-      <c r="G53" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="H53" s="3">
-        <v>1250</v>
-      </c>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
-      <c r="P53" s="3"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
-      <c r="P54" s="3"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1635,12 +1431,219 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{851CD717-A060-4A7E-8192-FC289E26CF5C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>111</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3">
+        <v>7102020</v>
+      </c>
+      <c r="E4" s="3">
+        <v>100</v>
+      </c>
+      <c r="F4" s="3">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="L4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="E5" s="3">
+        <v>110</v>
+      </c>
+      <c r="F5" s="3">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1300</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="E6" s="3">
+        <v>111</v>
+      </c>
+      <c r="F6" s="3">
+        <v>16</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1200</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="E7" s="3">
+        <v>115</v>
+      </c>
+      <c r="F7" s="3">
+        <v>20</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1250</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aumente mas bases de datos y expandi  las ya exstentes
añadí bases de datos recursivos y otras bases de datos
</commit_message>
<xml_diff>
--- a/mapeo.xlsx
+++ b/mapeo.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\base de datos proyectos\base-de-datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C991818F-6C18-48EF-9258-2AA87E080809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEAA9AD-6656-458B-A558-C86A0DAF5524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ofertas de materias" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="a">Sheet1!$XDP$18</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="141">
   <si>
     <t>PELICULA</t>
   </si>
@@ -332,6 +333,126 @@
   </si>
   <si>
     <t>stark</t>
+  </si>
+  <si>
+    <t>DOCENTE</t>
+  </si>
+  <si>
+    <t>GRUPO</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>MATERIA</t>
+  </si>
+  <si>
+    <t>SIGLA</t>
+  </si>
+  <si>
+    <t>CODIGOD</t>
+  </si>
+  <si>
+    <t>SIGLAM</t>
+  </si>
+  <si>
+    <t>introduccion a la informatica</t>
+  </si>
+  <si>
+    <t>INF 110</t>
+  </si>
+  <si>
+    <t>INF 119</t>
+  </si>
+  <si>
+    <t>estructuras discretas</t>
+  </si>
+  <si>
+    <t>Josue Veizaga</t>
+  </si>
+  <si>
+    <t>Carlos miranda</t>
+  </si>
+  <si>
+    <t>Juan Carlos Contreras</t>
+  </si>
+  <si>
+    <t>Kathime Gutierrez</t>
+  </si>
+  <si>
+    <t>INF 312</t>
+  </si>
+  <si>
+    <t>base de datos 1</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>SZ</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>INF312</t>
+  </si>
+  <si>
+    <t>INF 552</t>
+  </si>
+  <si>
+    <t>Arquitectura de software</t>
+  </si>
+  <si>
+    <t>HORARIO</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>horario inicial</t>
+  </si>
+  <si>
+    <t>horario final</t>
+  </si>
+  <si>
+    <t>TIENE</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>LUNES</t>
+  </si>
+  <si>
+    <t>MIERCOLES</t>
+  </si>
+  <si>
+    <t>VIERNES</t>
+  </si>
+  <si>
+    <t>MARTES</t>
+  </si>
+  <si>
+    <t>JUEVES</t>
+  </si>
+  <si>
+    <t>IDgrupo</t>
+  </si>
+  <si>
+    <t>IDhorario</t>
   </si>
 </sst>
 </file>
@@ -398,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -406,6 +527,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1433,7 +1555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{851CD717-A060-4A7E-8192-FC289E26CF5C}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+    <sheetView zoomScale="77" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1646,4 +1768,525 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5711E3ED-E077-4C15-976E-A88B0DB6076E}">
+  <dimension ref="A1:S18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" t="s">
+        <v>126</v>
+      </c>
+      <c r="R1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" t="s">
+        <v>130</v>
+      </c>
+      <c r="P2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>111</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="3">
+        <v>111</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="O4" s="6">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="R4" s="3">
+        <v>1</v>
+      </c>
+      <c r="S4" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>222</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="3">
+        <v>333</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M5" s="3">
+        <v>2</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="O5" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="R5" s="3">
+        <v>1</v>
+      </c>
+      <c r="S5" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>333</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="3">
+        <v>222</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="M6" s="3">
+        <v>3</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="O6" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P6" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="R6" s="3">
+        <v>2</v>
+      </c>
+      <c r="S6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>444</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="3">
+        <v>111</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="M7" s="3">
+        <v>4</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="O7" s="6">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P7" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="R7" s="3">
+        <v>2</v>
+      </c>
+      <c r="S7" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="3">
+        <v>111</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="3">
+        <v>5</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="O8" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="P8" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="R8" s="3">
+        <v>2</v>
+      </c>
+      <c r="S8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D9" s="7">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="7">
+        <v>111</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="M9" s="3">
+        <v>6</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="O9" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P9" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="R9" s="3">
+        <v>4</v>
+      </c>
+      <c r="S9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="M10" s="3">
+        <v>7</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="O10" s="6">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="R10" s="3">
+        <v>4</v>
+      </c>
+      <c r="S10" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="M11" s="3">
+        <v>8</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="O11" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="P11" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="R11" s="3">
+        <v>4</v>
+      </c>
+      <c r="S11" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="M12" s="3">
+        <v>9</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="O12" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P12" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="R12" s="3">
+        <v>3</v>
+      </c>
+      <c r="S12" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="M13" s="3">
+        <v>10</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="O13" s="6">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P13" s="6">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="R13" s="3">
+        <v>3</v>
+      </c>
+      <c r="S13" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="M14" s="3">
+        <v>11</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="O14" s="6">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="P14" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="R14" s="3">
+        <v>5</v>
+      </c>
+      <c r="S14" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="M15" s="3">
+        <v>12</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O15" s="6">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P15" s="6">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="R15" s="3">
+        <v>5</v>
+      </c>
+      <c r="S15" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="M16" s="3">
+        <v>13</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O16" s="6">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="P16" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="R16" s="3">
+        <v>6</v>
+      </c>
+      <c r="S16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="13:19" x14ac:dyDescent="0.3">
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="R17" s="3">
+        <v>6</v>
+      </c>
+      <c r="S17" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="13:19" x14ac:dyDescent="0.3">
+      <c r="R18" s="7">
+        <v>6</v>
+      </c>
+      <c r="S18" s="7">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>